<commit_message>
working on the JS file, building the logic for the calculate, also creating the table
</commit_message>
<xml_diff>
--- a/Practica Javascript/Simulador de créditos/resources/formulas.xlsx
+++ b/Practica Javascript/Simulador de créditos/resources/formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Cmder\projects\basics-frontend\Practica Javascript\Simulador de créditos\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA3EA93-3C82-4EB2-84EC-8C5B668625DE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50697D9C-BE75-4EC5-A24A-E7264E386EAF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7980" xr2:uid="{CB1AFF6C-1354-4EAD-BC5E-AD4802EBC889}"/>
   </bookViews>
@@ -57,20 +57,20 @@
     <t>interes</t>
   </si>
   <si>
-    <t>salso</t>
-  </si>
-  <si>
     <t>Cuota = (Monto * (%MV x (1 + %MV) ^ n)) / ((1 + %MV) ^ n) - 1)</t>
   </si>
   <si>
     <t>k*(i*(1+i)^n))/((1+i)^n)-1)</t>
+  </si>
+  <si>
+    <t>saldo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +83,14 @@
       <color rgb="FF8C8C8C"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,12 +113,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,14 +437,14 @@
   <dimension ref="A1:I46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -454,7 +463,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1.2E-2</v>
+        <v>1.15E-2</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -470,10 +479,26 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
+      <c r="E3">
+        <f>(1+0.0115)^B3</f>
+        <v>1.4921278924351102</v>
+      </c>
+      <c r="F3">
+        <f>1.15/100</f>
+        <v>1.15E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f>(1+B2)^B3</f>
+        <v>1.4921278924351102</v>
+      </c>
+      <c r="F4">
+        <f>(F3+1)^B3</f>
+        <v>1.4921278924351102</v>
+      </c>
       <c r="H4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -482,7 +507,7 @@
       </c>
       <c r="B5" s="2">
         <f>+PMT(B2,B3,-B1)</f>
-        <v>281270.46750894765</v>
+        <v>278943.2751408855</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -491,7 +516,7 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <f>(B1*B2*((1+B2)^B3))/(((1+B2)^B3)-1)</f>
-        <v>281270.46750894777</v>
+        <v>278943.27514088363</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -505,10 +530,10 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -526,32 +551,33 @@
       </c>
       <c r="C10" s="2">
         <f>+$B$5-D10</f>
-        <v>185270.46750894765</v>
+        <v>186943.2751408855</v>
       </c>
       <c r="D10" s="2">
         <f>+E9*$B$2</f>
-        <v>96000</v>
+        <v>92000</v>
       </c>
       <c r="E10" s="2">
         <f>+E9-C10</f>
-        <v>7814729.5324910525</v>
-      </c>
+        <v>7813056.7248591147</v>
+      </c>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" s="2">
-        <f t="shared" ref="C11:C44" si="0">+$B$5-D11</f>
-        <v>187493.71311905503</v>
+        <f>+$B$5-D11</f>
+        <v>189093.1228050057</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" ref="D11:D44" si="1">+E10*$B$2</f>
-        <v>93776.754389892638</v>
+        <f>+E10*$B$2</f>
+        <v>89850.152335879815</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" ref="E11:E44" si="2">+E10-C11</f>
-        <v>7627235.8193719974</v>
+        <f t="shared" ref="E11:E44" si="0">+E10-C11</f>
+        <v>7623963.6020541089</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -559,16 +585,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="2">
-        <f t="shared" si="0"/>
-        <v>189743.63767648366</v>
+        <f t="shared" ref="C11:C44" si="1">+$B$5-D12</f>
+        <v>191267.69371726323</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" si="1"/>
-        <v>91526.829832463976</v>
+        <f t="shared" ref="D11:D44" si="2">+E11*$B$2</f>
+        <v>87675.58142362225</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="2"/>
-        <v>7437492.1816955134</v>
+        <f t="shared" si="0"/>
+        <v>7432695.9083368452</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -576,16 +602,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="2">
-        <f t="shared" si="0"/>
-        <v>192020.5613286015</v>
+        <f t="shared" si="1"/>
+        <v>193467.27219501178</v>
       </c>
       <c r="D13" s="2">
-        <f t="shared" si="1"/>
-        <v>89249.906180346166</v>
+        <f t="shared" si="2"/>
+        <v>85476.002945873712</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" si="2"/>
-        <v>7245471.6203669123</v>
+        <f t="shared" si="0"/>
+        <v>7239228.6361418338</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -593,16 +619,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="2">
-        <f t="shared" si="0"/>
-        <v>194324.80806454469</v>
+        <f t="shared" si="1"/>
+        <v>195692.14582525441</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" si="1"/>
-        <v>86945.659444402947</v>
+        <f t="shared" si="2"/>
+        <v>83251.129315631086</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" si="2"/>
-        <v>7051146.8123023678</v>
+        <f t="shared" si="0"/>
+        <v>7043536.4903165791</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -610,16 +636,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" si="0"/>
-        <v>196656.70576131923</v>
+        <f t="shared" si="1"/>
+        <v>197942.60550224484</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" si="1"/>
-        <v>84613.761747628421</v>
+        <f>+E14*$B$2</f>
+        <v>81000.669638640655</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="2"/>
-        <v>6854490.1065410487</v>
+        <f t="shared" si="0"/>
+        <v>6845593.8848143341</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -627,16 +653,16 @@
         <v>7</v>
       </c>
       <c r="C16" s="2">
-        <f t="shared" si="0"/>
-        <v>199016.58623045508</v>
+        <f>+$B$5-D16</f>
+        <v>200218.94546552066</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="1"/>
-        <v>82253.881278492583</v>
+        <f t="shared" si="2"/>
+        <v>78724.329675364846</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="2"/>
-        <v>6655473.5203105938</v>
+        <f t="shared" si="0"/>
+        <v>6645374.9393488131</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -644,16 +670,16 @@
         <v>8</v>
       </c>
       <c r="C17" s="2">
-        <f t="shared" si="0"/>
-        <v>201404.7852652205</v>
+        <f t="shared" si="1"/>
+        <v>202521.46333837416</v>
       </c>
       <c r="D17" s="2">
-        <f t="shared" si="1"/>
-        <v>79865.682243727133</v>
+        <f t="shared" si="2"/>
+        <v>76421.811802511351</v>
       </c>
       <c r="E17" s="2">
-        <f t="shared" si="2"/>
-        <v>6454068.7350453734</v>
+        <f t="shared" si="0"/>
+        <v>6442853.476010439</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -661,16 +687,16 @@
         <v>9</v>
       </c>
       <c r="C18" s="2">
-        <f t="shared" si="0"/>
-        <v>203821.64268840317</v>
+        <f t="shared" si="1"/>
+        <v>204850.46016676544</v>
       </c>
       <c r="D18" s="2">
-        <f t="shared" si="1"/>
-        <v>77448.824820544483</v>
+        <f t="shared" si="2"/>
+        <v>74092.814974120047</v>
       </c>
       <c r="E18" s="2">
-        <f t="shared" si="2"/>
-        <v>6250247.0923569705</v>
+        <f t="shared" si="0"/>
+        <v>6238003.0158436736</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -678,16 +704,16 @@
         <v>10</v>
       </c>
       <c r="C19" s="2">
-        <f t="shared" si="0"/>
-        <v>206267.502400664</v>
+        <f t="shared" si="1"/>
+        <v>207206.24045868326</v>
       </c>
       <c r="D19" s="2">
-        <f t="shared" si="1"/>
-        <v>75002.96510828365</v>
+        <f t="shared" si="2"/>
+        <v>71737.03468220224</v>
       </c>
       <c r="E19" s="2">
-        <f t="shared" si="2"/>
-        <v>6043979.5899563069</v>
+        <f t="shared" si="0"/>
+        <v>6030796.7753849905</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -695,16 +721,16 @@
         <v>11</v>
       </c>
       <c r="C20" s="2">
-        <f t="shared" si="0"/>
-        <v>208742.71242947195</v>
+        <f t="shared" si="1"/>
+        <v>209589.1122239581</v>
       </c>
       <c r="D20" s="2">
-        <f t="shared" si="1"/>
-        <v>72527.755079475683</v>
+        <f t="shared" si="2"/>
+        <v>69354.162916927395</v>
       </c>
       <c r="E20" s="2">
-        <f t="shared" si="2"/>
-        <v>5835236.8775268346</v>
+        <f t="shared" si="0"/>
+        <v>5821207.6631610328</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -712,16 +738,16 @@
         <v>12</v>
       </c>
       <c r="C21" s="2">
-        <f t="shared" si="0"/>
-        <v>211247.62497862562</v>
+        <f t="shared" si="1"/>
+        <v>211999.38701453363</v>
       </c>
       <c r="D21" s="2">
-        <f t="shared" si="1"/>
-        <v>70022.842530322014</v>
+        <f t="shared" si="2"/>
+        <v>66943.888126351871</v>
       </c>
       <c r="E21" s="2">
-        <f t="shared" si="2"/>
-        <v>5623989.2525482094</v>
+        <f t="shared" si="0"/>
+        <v>5609208.2761464994</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -729,16 +755,16 @@
         <v>13</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" si="0"/>
-        <v>213782.59647836915</v>
+        <f t="shared" si="1"/>
+        <v>214437.37996520076</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="1"/>
-        <v>67487.871030578521</v>
+        <f t="shared" si="2"/>
+        <v>64505.895175684745</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" si="2"/>
-        <v>5410206.6560698403</v>
+        <f t="shared" si="0"/>
+        <v>5394770.8961812984</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -746,16 +772,16 @@
         <v>14</v>
       </c>
       <c r="C23" s="2">
-        <f t="shared" si="0"/>
-        <v>216347.98763610958</v>
+        <f t="shared" si="1"/>
+        <v>216903.40983480058</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" si="1"/>
-        <v>64922.479872838085</v>
+        <f t="shared" si="2"/>
+        <v>62039.865306084932</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" si="2"/>
-        <v>5193858.6684337305</v>
+        <f t="shared" si="0"/>
+        <v>5177867.4863464981</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -763,16 +789,16 @@
         <v>15</v>
       </c>
       <c r="C24" s="2">
-        <f t="shared" si="0"/>
-        <v>218944.16348774289</v>
+        <f t="shared" si="1"/>
+        <v>219397.79904790077</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="1"/>
-        <v>62326.304021204764</v>
+        <f t="shared" si="2"/>
+        <v>59545.476092984725</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="2"/>
-        <v>4974914.5049459878</v>
+        <f t="shared" si="0"/>
+        <v>4958469.6872985978</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -780,16 +806,16 @@
         <v>16</v>
       </c>
       <c r="C25" s="2">
-        <f t="shared" si="0"/>
-        <v>221571.49344959579</v>
+        <f t="shared" si="1"/>
+        <v>221920.87373695162</v>
       </c>
       <c r="D25" s="2">
-        <f t="shared" si="1"/>
-        <v>59698.974059351858</v>
+        <f t="shared" si="2"/>
+        <v>57022.401403933873</v>
       </c>
       <c r="E25" s="2">
-        <f t="shared" si="2"/>
-        <v>4753343.0114963921</v>
+        <f t="shared" si="0"/>
+        <v>4736548.8135616463</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -797,16 +823,16 @@
         <v>17</v>
       </c>
       <c r="C26" s="2">
-        <f t="shared" si="0"/>
-        <v>224230.35137099095</v>
+        <f t="shared" si="1"/>
+        <v>224472.96378492657</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="1"/>
-        <v>57040.116137956706</v>
+        <f t="shared" si="2"/>
+        <v>54470.311355958933</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="2"/>
-        <v>4529112.6601254009</v>
+        <f t="shared" si="0"/>
+        <v>4512075.8497767197</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -814,16 +840,16 @@
         <v>18</v>
       </c>
       <c r="C27" s="2">
-        <f t="shared" si="0"/>
-        <v>226921.11558744282</v>
+        <f t="shared" si="1"/>
+        <v>227054.40286845324</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="1"/>
-        <v>54349.351921504815</v>
+        <f t="shared" si="2"/>
+        <v>51888.872272432272</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" si="2"/>
-        <v>4302191.5445379578</v>
+        <f t="shared" si="0"/>
+        <v>4285021.4469082663</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -831,16 +857,16 @@
         <v>19</v>
       </c>
       <c r="C28" s="2">
-        <f t="shared" si="0"/>
-        <v>229644.16897449218</v>
+        <f t="shared" si="1"/>
+        <v>229665.52850144042</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="1"/>
-        <v>51626.298534455491</v>
+        <f t="shared" si="2"/>
+        <v>49277.74663944506</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="2"/>
-        <v>4072547.3755634655</v>
+        <f t="shared" si="0"/>
+        <v>4055355.918406826</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -848,16 +874,16 @@
         <v>20</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" si="0"/>
-        <v>232399.89900218608</v>
+        <f t="shared" si="1"/>
+        <v>232306.68207920701</v>
       </c>
       <c r="D29" s="2">
-        <f t="shared" si="1"/>
-        <v>48870.568506761585</v>
+        <f t="shared" si="2"/>
+        <v>46636.593061678497</v>
       </c>
       <c r="E29" s="2">
-        <f t="shared" si="2"/>
-        <v>3840147.4765612795</v>
+        <f t="shared" si="0"/>
+        <v>3823049.2363276188</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -865,16 +891,16 @@
         <v>21</v>
       </c>
       <c r="C30" s="2">
-        <f t="shared" si="0"/>
-        <v>235188.69779021229</v>
+        <f t="shared" si="1"/>
+        <v>234978.2089231179</v>
       </c>
       <c r="D30" s="2">
-        <f t="shared" si="1"/>
-        <v>46081.769718735355</v>
+        <f t="shared" si="2"/>
+        <v>43965.066217767613</v>
       </c>
       <c r="E30" s="2">
-        <f t="shared" si="2"/>
-        <v>3604958.778771067</v>
+        <f t="shared" si="0"/>
+        <v>3588071.0274045011</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -882,16 +908,16 @@
         <v>22</v>
       </c>
       <c r="C31" s="2">
-        <f t="shared" si="0"/>
-        <v>238010.96216369484</v>
+        <f t="shared" si="1"/>
+        <v>237680.45832573372</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" si="1"/>
-        <v>43259.505345252808</v>
+        <f t="shared" si="2"/>
+        <v>41262.81681515176</v>
       </c>
       <c r="E31" s="2">
-        <f t="shared" si="2"/>
-        <v>3366947.8166073724</v>
+        <f t="shared" si="0"/>
+        <v>3350390.5690787672</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
@@ -899,16 +925,16 @@
         <v>23</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" si="0"/>
-        <v>240867.09370965918</v>
+        <f t="shared" si="1"/>
+        <v>240413.78359647968</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" si="1"/>
-        <v>40403.373799288471</v>
+        <f t="shared" si="2"/>
+        <v>38529.491544405821</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="2"/>
-        <v>3126080.7228977131</v>
+        <f t="shared" si="0"/>
+        <v>3109976.7854822874</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
@@ -916,16 +942,16 @@
         <v>24</v>
       </c>
       <c r="C33" s="2">
-        <f t="shared" si="0"/>
-        <v>243757.49883417509</v>
+        <f t="shared" si="1"/>
+        <v>243178.5421078392</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" si="1"/>
-        <v>37512.968674772557</v>
+        <f t="shared" si="2"/>
+        <v>35764.733033046301</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="2"/>
-        <v>2882323.224063538</v>
+        <f t="shared" si="0"/>
+        <v>2866798.2433744483</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -933,16 +959,16 @@
         <v>25</v>
       </c>
       <c r="C34" s="2">
-        <f t="shared" si="0"/>
-        <v>246682.58882018519</v>
+        <f t="shared" si="1"/>
+        <v>245975.09534207935</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" si="1"/>
-        <v>34587.878688762459</v>
+        <f t="shared" si="2"/>
+        <v>32968.179798806152</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="2"/>
-        <v>2635640.635243353</v>
+        <f t="shared" si="0"/>
+        <v>2620823.1480323691</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
@@ -950,16 +976,16 @@
         <v>26</v>
       </c>
       <c r="C35" s="2">
-        <f t="shared" si="0"/>
-        <v>249642.77988602742</v>
+        <f t="shared" si="1"/>
+        <v>248803.80893851325</v>
       </c>
       <c r="D35" s="2">
-        <f t="shared" si="1"/>
-        <v>31627.687622920235</v>
+        <f t="shared" si="2"/>
+        <v>30139.466202372245</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="2"/>
-        <v>2385997.8553573256</v>
+        <f t="shared" si="0"/>
+        <v>2372019.339093856</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -967,16 +993,16 @@
         <v>27</v>
       </c>
       <c r="C36" s="2">
-        <f t="shared" si="0"/>
-        <v>252638.49324465974</v>
+        <f t="shared" si="1"/>
+        <v>251665.05274130616</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" si="1"/>
-        <v>28631.974264287906</v>
+        <f t="shared" si="2"/>
+        <v>27278.222399579343</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="2"/>
-        <v>2133359.362112666</v>
+        <f t="shared" si="0"/>
+        <v>2120354.2863525497</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -984,16 +1010,16 @@
         <v>28</v>
       </c>
       <c r="C37" s="2">
-        <f t="shared" si="0"/>
-        <v>255670.15516359566</v>
+        <f t="shared" si="1"/>
+        <v>254559.20084783118</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" si="1"/>
-        <v>25600.312345351991</v>
+        <f t="shared" si="2"/>
+        <v>24384.07429305432</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" si="2"/>
-        <v>1877689.2069490703</v>
+        <f t="shared" si="0"/>
+        <v>1865795.0855047186</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -1001,16 +1027,16 @@
         <v>29</v>
       </c>
       <c r="C38" s="2">
-        <f t="shared" si="0"/>
-        <v>258738.19702555879</v>
+        <f t="shared" si="1"/>
+        <v>257486.63165758122</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="1"/>
-        <v>22532.270483388846</v>
+        <f t="shared" si="2"/>
+        <v>21456.643483304262</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" si="2"/>
-        <v>1618951.0099235117</v>
+        <f t="shared" si="0"/>
+        <v>1608308.4538471373</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
@@ -1018,16 +1044,16 @@
         <v>30</v>
       </c>
       <c r="C39" s="2">
-        <f t="shared" si="0"/>
-        <v>261843.05538986551</v>
+        <f t="shared" si="1"/>
+        <v>260447.72792164341</v>
       </c>
       <c r="D39" s="2">
-        <f t="shared" si="1"/>
-        <v>19427.412119082139</v>
+        <f t="shared" si="2"/>
+        <v>18495.547219242078</v>
       </c>
       <c r="E39" s="2">
-        <f t="shared" si="2"/>
-        <v>1357107.9545336461</v>
+        <f t="shared" si="0"/>
+        <v>1347860.725925494</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
@@ -1035,16 +1061,16 @@
         <v>31</v>
       </c>
       <c r="C40" s="2">
-        <f t="shared" si="0"/>
-        <v>264985.17205454392</v>
+        <f t="shared" si="1"/>
+        <v>263442.87679274229</v>
       </c>
       <c r="D40" s="2">
-        <f t="shared" si="1"/>
-        <v>16285.295454403753</v>
+        <f t="shared" si="2"/>
+        <v>15500.398348143181</v>
       </c>
       <c r="E40" s="2">
-        <f t="shared" si="2"/>
-        <v>1092122.7824791023</v>
+        <f t="shared" si="0"/>
+        <v>1084417.8491327516</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
@@ -1052,16 +1078,16 @@
         <v>32</v>
       </c>
       <c r="C41" s="2">
-        <f t="shared" si="0"/>
-        <v>268164.99411919841</v>
+        <f t="shared" si="1"/>
+        <v>266472.46987585886</v>
       </c>
       <c r="D41" s="2">
-        <f t="shared" si="1"/>
-        <v>13105.473389749228</v>
+        <f t="shared" si="2"/>
+        <v>12470.805265026644</v>
       </c>
       <c r="E41" s="2">
-        <f t="shared" si="2"/>
-        <v>823957.78835990385</v>
+        <f>+E40-C41</f>
+        <v>817945.37925689272</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
@@ -1069,16 +1095,16 @@
         <v>33</v>
       </c>
       <c r="C42" s="2">
-        <f t="shared" si="0"/>
-        <v>271382.97404862882</v>
+        <f t="shared" si="1"/>
+        <v>269536.90327943122</v>
       </c>
       <c r="D42" s="2">
-        <f t="shared" si="1"/>
-        <v>9887.4934603188467</v>
+        <f t="shared" si="2"/>
+        <v>9406.3718614542668</v>
       </c>
       <c r="E42" s="2">
-        <f t="shared" si="2"/>
-        <v>552574.81431127503</v>
+        <f t="shared" si="0"/>
+        <v>548408.47597746155</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
@@ -1086,16 +1112,16 @@
         <v>34</v>
       </c>
       <c r="C43" s="2">
-        <f t="shared" si="0"/>
-        <v>274639.56973721232</v>
+        <f t="shared" si="1"/>
+        <v>272636.57766714471</v>
       </c>
       <c r="D43" s="2">
-        <f t="shared" si="1"/>
-        <v>6630.8977717353</v>
+        <f t="shared" si="2"/>
+        <v>6306.6974737408082</v>
       </c>
       <c r="E43" s="2">
-        <f t="shared" si="2"/>
-        <v>277935.2445740627</v>
+        <f t="shared" si="0"/>
+        <v>275771.89831031684</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
@@ -1103,22 +1129,22 @@
         <v>35</v>
       </c>
       <c r="C44" s="2">
-        <f t="shared" si="0"/>
-        <v>277935.24457405892</v>
+        <f t="shared" si="1"/>
+        <v>275771.89831031684</v>
       </c>
       <c r="D44" s="2">
-        <f t="shared" si="1"/>
-        <v>3335.2229348887527</v>
+        <f t="shared" si="2"/>
+        <v>3171.3768305686435</v>
       </c>
       <c r="E44" s="2">
-        <f t="shared" si="2"/>
-        <v>3.7834979593753815E-9</v>
+        <f>+E43-C44</f>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f>SUM(C10:C45)</f>
-        <v>7999999.9999999972</v>
+        <v>8000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>